<commit_message>
xx git commit -m xx
xit
a
</commit_message>
<xml_diff>
--- a/admin/production/uploads/filemau.xlsx
+++ b/admin/production/uploads/filemau.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\thlogistics\admin\production\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1464,13 +1464,13 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>350373</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>155111</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>964076</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>895350</xdr:rowOff>
+      <xdr:rowOff>768814</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1499,8 +1499,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1493373" y="3076575"/>
-          <a:ext cx="613703" cy="866775"/>
+          <a:off x="1493373" y="3203111"/>
+          <a:ext cx="613703" cy="613703"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1512,13 +1512,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>157770</xdr:colOff>
+      <xdr:colOff>292894</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>342900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1180492</xdr:colOff>
+      <xdr:colOff>1045368</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>1095374</xdr:rowOff>
     </xdr:to>
@@ -1552,8 +1552,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1300770" y="4352925"/>
-          <a:ext cx="1022722" cy="752474"/>
+          <a:off x="1435894" y="4352925"/>
+          <a:ext cx="752474" cy="752474"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1565,13 +1565,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>194268</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>270468</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1181100</xdr:colOff>
+      <xdr:colOff>986832</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>1063032</xdr:rowOff>
     </xdr:to>
@@ -1605,8 +1605,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1143000" y="5680668"/>
-          <a:ext cx="1181100" cy="792564"/>
+          <a:off x="1337268" y="5680668"/>
+          <a:ext cx="792564" cy="792564"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1916,7 +1916,7 @@
   <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>